<commit_message>
fixed bug null urls
</commit_message>
<xml_diff>
--- a/down_send/errors.xlsx
+++ b/down_send/errors.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,21 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -330,13 +385,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>":null,"thumbhttps://m.media-amazon.com/images/I/51umk+HPQbL._AC_SR38,50_.jpg</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>iphone 7 negro</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
solved bug with / in filenames
</commit_message>
<xml_diff>
--- a/down_send/errors.xlsx
+++ b/down_send/errors.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -401,12 +401,48 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>no item appended</t>
+          <t>https://d1eh9yux7w8iql.cloudfront.net/product_images/413837_34622d71-7e56-4018-b00e-26298dea5124.jpg</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>https://www.fnac.es/Samsung-Galaxy-Fold-7-3-512GB-Negro-Telefono-movil-Smartphone/a7132771#omnsearchpos=11</t>
+          <t>iphone 12 pro max negro/grafito</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://d1eh9yux7w8iql.cloudfront.net/product_images/413837_81c85355-e6d5-47d7-b060-05c4d8968965.jpg</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>iphone 12 pro max negro/grafito</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://d1eh9yux7w8iql.cloudfront.net/product_images/413837_025f5c2e-e75f-4a13-b25e-d92c7dfd7e0b.jpg</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>iphone 12 pro max negro/grafito</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://d1eh9yux7w8iql.cloudfront.net/product_images/413837_fa07ef38-b2a1-44ae-ba4d-d5bf31ac39d1.jpg</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>iphone 12 pro max negro/grafito</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added logging function + complete list
</commit_message>
<xml_diff>
--- a/down_send/errors.xlsx
+++ b/down_send/errors.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -390,59 +390,59 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>https://d1eh9yux7w8iql.cloudfront.net/product_images/413837_34622d71-7e56-4018-b00e-26298dea5124.jpg</t>
+          <t>samsung galaxy fold negro</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>iphone 12 pro max negro/grafito</t>
+          <t>https://www.fnac.es/Samsung-Galaxy-Fold-7-3-512GB-Negro-Telefono-movil-Smartphone/a7132771#omnsearchpos=11</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://d1eh9yux7w8iql.cloudfront.net/product_images/413837_81c85355-e6d5-47d7-b060-05c4d8968965.jpg</t>
+          <t>iphone 12 pro max oro</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>iphone 12 pro max negro/grafito</t>
+          <t>https://www.backmarket.es/iphone-12-pro-max-128-gb-oro-libre-segunda-mano/413839.html#l=10</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://d1eh9yux7w8iql.cloudfront.net/product_images/413837_025f5c2e-e75f-4a13-b25e-d92c7dfd7e0b.jpg</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>iphone 12 pro max negro/grafito</t>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>samsung galaxy fold negro</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://www.fnac.es/Samsung-Galaxy-Fold-7-3-512GB-Negro-Telefono-movil-Smartphone/a7132771#omnsearchpos=11</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://d1eh9yux7w8iql.cloudfront.net/product_images/413837_fa07ef38-b2a1-44ae-ba4d-d5bf31ac39d1.jpg</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>iphone 12 pro max negro/grafito</t>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>iphone 12 pro max oro</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://www.backmarket.es/iphone-12-pro-max-128-gb-oro-libre-segunda-mano/413839.html#l=10</t>
         </is>
       </c>
     </row>

</xml_diff>